<commit_message>
its a long time not to commit
</commit_message>
<xml_diff>
--- a/gatte.xlsx
+++ b/gatte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0E4879-B85F-4066-AFFA-BB18E5DB9330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D284066B-34DE-4AE6-B7DF-E726F97B0D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6285" yWindow="2115" windowWidth="15165" windowHeight="11235" firstSheet="34" activeTab="37" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8085" yWindow="1680" windowWidth="15165" windowHeight="11235" firstSheet="35" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,8 @@
     <sheet name="2021-10-25" sheetId="41" r:id="rId36"/>
     <sheet name="2021-11-01" sheetId="42" r:id="rId37"/>
     <sheet name="2021-11-08" sheetId="43" r:id="rId38"/>
-    <sheet name="template" sheetId="35" r:id="rId39"/>
+    <sheet name="2021-11-15" sheetId="44" r:id="rId39"/>
+    <sheet name="template" sheetId="35" r:id="rId40"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="405">
   <si>
     <t>起始</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1661,6 +1662,26 @@
   </si>
   <si>
     <t>knn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>opencv-learn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c#-learn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>linux</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>linux-doc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git-host</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -30029,8 +30050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101EA6BF-CEB9-459F-8C65-D5FB0A3DEFF4}">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C39" activeCellId="1" sqref="C38 C39"/>
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -30069,7 +30090,7 @@
         <v>393</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D39" si="0">INT(ABS(B2-A2)*1440)</f>
+        <f t="shared" ref="D2:D41" si="0">INT(ABS(B2-A2)*1440)</f>
         <v>29</v>
       </c>
     </row>
@@ -30659,13 +30680,35 @@
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
+      <c r="A40" s="5">
+        <v>44513.428472222222</v>
+      </c>
+      <c r="B40" s="5">
+        <v>44513.459027777775</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
+      <c r="A41" s="5">
+        <v>44513.634722222225</v>
+      </c>
+      <c r="B41" s="5">
+        <v>44513.683333333334</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -30964,11 +31007,11 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A596D9-6FE7-4DE5-A4A1-43FCD86B01B8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9846F590-A4D1-4CDC-994A-3D3B35F2476E}">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -30998,235 +31041,590 @@
     </row>
     <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>44452.37222222222</v>
+        <v>44515.392361111109</v>
       </c>
       <c r="B2" s="5">
-        <v>44452.388888888891</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>346</v>
+        <v>44515.399305555555</v>
+      </c>
+      <c r="C2" s="1">
+        <v>78</v>
       </c>
       <c r="D2" s="1">
-        <f>INT(ABS(B2-A2)*1440)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+        <f t="shared" ref="D2:D34" si="0">INT(ABS(B2-A2)*1440)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>44515.399305555555</v>
+      </c>
+      <c r="B3" s="5">
+        <v>44515.425000000003</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
     <row r="4" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="5">
+        <v>44515.428472222222</v>
+      </c>
+      <c r="B4" s="5">
+        <v>44515.475694444445</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="5">
+        <v>44515.556944444441</v>
+      </c>
+      <c r="B5" s="5">
+        <v>44515.587500000001</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="5">
+        <v>44515.597222222219</v>
+      </c>
+      <c r="B6" s="5">
+        <v>44515.622916666667</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="5">
+        <v>44515.62777777778</v>
+      </c>
+      <c r="B7" s="5">
+        <v>44515.68472222222</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="5">
+        <v>44515.702777777777</v>
+      </c>
+      <c r="B8" s="5">
+        <v>44515.738888888889</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="5">
+        <v>44515.745138888888</v>
+      </c>
+      <c r="B9" s="5">
+        <v>44515.765277777777</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="5">
+        <v>44515.861111111109</v>
+      </c>
+      <c r="B10" s="5">
+        <v>44515.940972222219</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11" s="5">
+        <v>44516.370833333334</v>
+      </c>
+      <c r="B11" s="5">
+        <v>44516.447916666664</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12" s="5">
+        <v>44516.454861111109</v>
+      </c>
+      <c r="B12" s="5">
+        <v>44516.475694444445</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A13" s="5">
+        <v>44516.600694444445</v>
+      </c>
+      <c r="B13" s="5">
+        <v>44516.626388888886</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="A14" s="5">
+        <v>44516.629861111112</v>
+      </c>
+      <c r="B14" s="5">
+        <v>44516.677083333336</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="5">
+        <v>44516.678472222222</v>
+      </c>
+      <c r="B15" s="5">
+        <v>44516.68472222222</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="A16" s="5">
+        <v>44516.689583333333</v>
+      </c>
+      <c r="B16" s="5">
+        <v>44516.712500000001</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+    <row r="17" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>44516.715277777781</v>
+      </c>
+      <c r="B17" s="5">
+        <v>44516.734722222223</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+    <row r="18" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>44516.743750000001</v>
+      </c>
+      <c r="B18" s="5">
+        <v>44516.76666666667</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>44516.883333333331</v>
+      </c>
+      <c r="B19" s="5">
+        <v>44516.931944444441</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+    <row r="20" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>44516.950694444444</v>
+      </c>
+      <c r="B20" s="5">
+        <v>44516.955555555556</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+    <row r="21" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>44517.319444444445</v>
+      </c>
+      <c r="B21" s="5">
+        <v>44517.330555555556</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+    <row r="22" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>44517.361805555556</v>
+      </c>
+      <c r="B22" s="5">
+        <v>44517.428472222222</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+    <row r="23" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>44517.432638888888</v>
+      </c>
+      <c r="B23" s="5">
+        <v>44517.474999999999</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+    <row r="24" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>44517.575694444444</v>
+      </c>
+      <c r="B24" s="5">
+        <v>44517.615277777775</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+    <row r="25" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>44517.623611111114</v>
+      </c>
+      <c r="B25" s="5">
+        <v>44517.647916666669</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+    <row r="26" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>44517.668055555558</v>
+      </c>
+      <c r="B26" s="5">
+        <v>44517.727083333331</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+    <row r="27" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>44518.388194444444</v>
+      </c>
+      <c r="B27" s="5">
+        <v>44518.416666666664</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+    <row r="28" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>44518.421527777777</v>
+      </c>
+      <c r="B28" s="5">
+        <v>44518.474999999999</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+    <row r="29" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>44518.538194444445</v>
+      </c>
+      <c r="B29" s="5">
+        <v>44518.59097222222</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+    <row r="30" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>44518.594444444447</v>
+      </c>
+      <c r="B30" s="5">
+        <v>44518.661111111112</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+    <row r="31" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>44518.665972222225</v>
+      </c>
+      <c r="B31" s="5">
+        <v>44518.692361111112</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+    <row r="32" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>44518.704861111109</v>
+      </c>
+      <c r="B32" s="5">
+        <v>44518.728472222225</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+    <row r="33" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>44519.350694444445</v>
+      </c>
+      <c r="B33" s="5">
+        <v>44519.475694444445</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
+    <row r="34" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>44519.504861111112</v>
+      </c>
+      <c r="B34" s="5">
+        <v>44519.538888888892</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -31462,7 +31860,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4DB1EEFA-1E6D-4332-9B2A-4F1CCB416A2C}</x14:id>
+          <x14:id>{0C8E0C8C-67C0-4B87-8348-FE173DAC2A11}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -31473,7 +31871,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4DB1EEFA-1E6D-4332-9B2A-4F1CCB416A2C}">
+          <x14:cfRule type="dataBar" id="{0C8E0C8C-67C0-4B87-8348-FE173DAC2A11}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -31917,6 +32315,534 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{2A906CEB-2C87-499D-8E95-0B97CA577787}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A596D9-6FE7-4DE5-A4A1-43FCD86B01B8}">
+  <dimension ref="A1:E92"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="15.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>44452.37222222222</v>
+      </c>
+      <c r="B2" s="5">
+        <v>44452.388888888891</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D2" s="1">
+        <f>INT(ABS(B2-A2)*1440)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="3:5" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+    </row>
+    <row r="68" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+    </row>
+    <row r="78" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+    </row>
+    <row r="79" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+    </row>
+    <row r="80" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+    </row>
+    <row r="81" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+    </row>
+    <row r="82" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+    </row>
+    <row r="83" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+    </row>
+    <row r="84" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+    </row>
+    <row r="87" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+    </row>
+    <row r="88" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+    </row>
+    <row r="89" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+    </row>
+    <row r="91" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="3:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4DB1EEFA-1E6D-4332-9B2A-4F1CCB416A2C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4DB1EEFA-1E6D-4332-9B2A-4F1CCB416A2C}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>